<commit_message>
filled in lorem ipsum, finished subsec names
</commit_message>
<xml_diff>
--- a/documentation/timesheet_group4.xlsx
+++ b/documentation/timesheet_group4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usi365-my.sharepoint.com/personal/kerin_usi_ch/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kerinikolettnoemi/G4/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="216" documentId="8_{CC920DEC-777B-2D45-BCEC-F45C466A26FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3032ABFE-5F16-4B61-9B8B-AC29C6EECE5D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8BC20B-8B72-4442-BFE5-42DEB9DFF99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{44587F8E-F0B6-C848-BD56-AC9E293EC7A4}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{44587F8E-F0B6-C848-BD56-AC9E293EC7A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="117">
   <si>
     <t>NAME</t>
   </si>
@@ -378,6 +378,33 @@
   </si>
   <si>
     <t>11.10.</t>
+  </si>
+  <si>
+    <t>timesheet, meeting with kyle, group management</t>
+  </si>
+  <si>
+    <t>intro page plan, connections polishing, complete plan done</t>
+  </si>
+  <si>
+    <t>presentation</t>
+  </si>
+  <si>
+    <t>finished intro page, all is left to link pages</t>
+  </si>
+  <si>
+    <t>talked with the css leaders about progress, made an idea on how to connect the pages within the pages, talked to the css leaders about my plan</t>
+  </si>
+  <si>
+    <t>travel day, just talked to kyle about some admin stuff</t>
+  </si>
+  <si>
+    <t>intro page development, talking to the team members about deadlines, reminders, checking on progress</t>
+  </si>
+  <si>
+    <t>checking on progress, started writing the introductions for topics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">travel day </t>
   </si>
 </sst>
 </file>
@@ -845,45 +872,45 @@
   <dimension ref="A1:AB19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="W1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z6" sqref="Z6"/>
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="7" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="31.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="107.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="70.75" customWidth="1"/>
-    <col min="13" max="13" width="36.75" style="2" customWidth="1"/>
+    <col min="9" max="9" width="26.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="107.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="70.6640625" customWidth="1"/>
+    <col min="13" max="13" width="36.6640625" style="2" customWidth="1"/>
     <col min="14" max="14" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="20.6640625" style="2" customWidth="1"/>
     <col min="16" max="16" width="17.5" style="2" customWidth="1"/>
-    <col min="17" max="17" width="42.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="50.125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="14.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="35.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="42.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="50.1640625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="35.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="18" style="2" customWidth="1"/>
-    <col min="22" max="22" width="11.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="70.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="70.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.6640625" style="1" customWidth="1"/>
     <col min="26" max="26" width="86" style="2" customWidth="1"/>
     <col min="27" max="27" width="36" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="29.375" style="2" customWidth="1"/>
+    <col min="28" max="28" width="29.33203125" style="2" customWidth="1"/>
     <col min="29" max="16383" width="11" style="2"/>
     <col min="16384" max="16384" width="11" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" ht="25.5">
+    <row r="1" spans="1:28" s="1" customFormat="1" ht="30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -969,7 +996,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="1" customFormat="1" ht="25.5">
+    <row r="2" spans="1:28" s="1" customFormat="1" ht="30">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -1047,7 +1074,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="13.5">
+    <row r="3" spans="1:28" ht="15">
       <c r="B3" s="3" t="s">
         <v>53</v>
       </c>
@@ -1100,7 +1127,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" ht="16">
       <c r="B4" s="3" t="s">
         <v>70</v>
       </c>
@@ -1147,7 +1174,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="26.25">
+    <row r="5" spans="1:28" ht="27">
       <c r="B5" s="3" t="s">
         <v>85</v>
       </c>
@@ -1157,6 +1184,9 @@
       <c r="F5" s="11" t="s">
         <v>62</v>
       </c>
+      <c r="J5" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="M5" s="2" t="s">
         <v>87</v>
       </c>
@@ -1170,7 +1200,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" ht="16">
       <c r="B6" s="3" t="s">
         <v>91</v>
       </c>
@@ -1180,71 +1210,95 @@
       <c r="F6" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="J6" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="R6" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:28" ht="16">
       <c r="B7" s="3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="8" spans="1:28">
+      <c r="J7" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="16">
       <c r="B8" s="3" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="9" spans="1:28">
+      <c r="J8" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="16">
       <c r="B9" s="3" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="10" spans="1:28">
+      <c r="J9" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="16">
       <c r="B10" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="11" spans="1:28">
+      <c r="J10" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="16">
       <c r="B11" s="3" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="12" spans="1:28">
+      <c r="J11" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="16">
       <c r="B12" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="13" spans="1:28">
+      <c r="J12" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="16">
       <c r="B13" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="14" spans="1:28">
+      <c r="J13" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="16">
       <c r="B14" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:28" ht="16">
       <c r="B15" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:28" ht="16">
       <c r="B16" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="2:2" ht="16">
       <c r="B17" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="2:2">
+    <row r="18" spans="2:2" ht="16">
       <c r="B18" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="2:2">
+    <row r="19" spans="2:2" ht="16">
       <c r="B19" s="3" t="s">
         <v>107</v>
       </c>

</xml_diff>